<commit_message>
Update: Se modifica estatus origen en padron vales y se agrega módulo para auditoria
</commit_message>
<xml_diff>
--- a/public/archivos/formatoReporteNominaCalentador.xlsx
+++ b/public/archivos/formatoReporteNominaCalentador.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10917"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/diegolopez/Documents/GitProyect/vales/apivales/public/archivos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C29AEE5-FBCF-084E-BA6E-A361999275B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{190E09E9-5FA4-624B-8615-5C31AAC955BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Solicitudes Vales Grandeza" sheetId="1" r:id="rId1"/>
+    <sheet name="Solicitudes CalentadoresSolares" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Solicitudes Vales Grandeza'!$A$2:$U$24</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Solicitudes Vales Grandeza'!$1:$10</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Solicitudes CalentadoresSolares'!$A$2:$U$24</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Solicitudes CalentadoresSolares'!$1:$10</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>NO.</t>
   </si>
@@ -121,6 +121,9 @@
   </si>
   <si>
     <t>Fecha Actualizo</t>
+  </si>
+  <si>
+    <t>FolioImpulso</t>
   </si>
 </sst>
 </file>
@@ -630,8 +633,8 @@
   </sheetPr>
   <dimension ref="A1:AH15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="137" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="137" workbookViewId="0">
+      <selection activeCell="AC10" sqref="AC10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -662,7 +665,8 @@
     <col min="26" max="26" width="15.83203125" style="7" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="34.1640625" style="7" customWidth="1"/>
     <col min="28" max="28" width="16.5" style="7" bestFit="1" customWidth="1"/>
-    <col min="29" max="16384" width="11.5" style="7"/>
+    <col min="29" max="29" width="35" style="7" customWidth="1"/>
+    <col min="30" max="16384" width="11.5" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -956,6 +960,9 @@
       </c>
       <c r="AB10" s="3" t="s">
         <v>27</v>
+      </c>
+      <c r="AC10" s="3" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Add: Se agrega módulo para control de usuarios
</commit_message>
<xml_diff>
--- a/public/archivos/formatoReporteNominaCalentador.xlsx
+++ b/public/archivos/formatoReporteNominaCalentador.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10414"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/diegolopez/Documents/GitProyect/vales/apivales/public/archivos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{190E09E9-5FA4-624B-8615-5C31AAC955BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E4CEB68-998D-134B-974D-607019CD06D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Solicitudes CalentadoresSolares" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>NO.</t>
   </si>
@@ -124,6 +124,9 @@
   </si>
   <si>
     <t>FolioImpulso</t>
+  </si>
+  <si>
+    <t>Ejercicio</t>
   </si>
 </sst>
 </file>
@@ -633,8 +636,8 @@
   </sheetPr>
   <dimension ref="A1:AH15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="137" workbookViewId="0">
-      <selection activeCell="AC10" sqref="AC10"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="137" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -964,6 +967,9 @@
       <c r="AC10" s="3" t="s">
         <v>28</v>
       </c>
+      <c r="AD10" s="3" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="11" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>

</xml_diff>

<commit_message>
Upd: Cambios de documentos para acuse y solicitud
</commit_message>
<xml_diff>
--- a/public/archivos/formatoReporteNominaCalentador.xlsx
+++ b/public/archivos/formatoReporteNominaCalentador.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10811"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/diegolopez/Documents/GitProyect/vales/apivales/public/archivos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E4CEB68-998D-134B-974D-607019CD06D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A043F19C-D7F3-A244-A7CB-D39A88937E39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Solicitudes CalentadoresSolares" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Solicitudes CalentadoresSolares'!$A$2:$U$24</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Solicitudes CalentadoresSolares'!$A$2:$V$24</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Solicitudes CalentadoresSolares'!$1:$10</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>NO.</t>
   </si>
@@ -127,6 +127,9 @@
   </si>
   <si>
     <t>Ejercicio</t>
+  </si>
+  <si>
+    <t>CveInegiLocalidad</t>
   </si>
 </sst>
 </file>
@@ -634,10 +637,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AH15"/>
+  <dimension ref="A1:AI15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="137" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="137" workbookViewId="0">
+      <selection activeCell="S10" sqref="S10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -657,22 +660,22 @@
     <col min="15" max="15" width="9" style="5" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="9" style="5" customWidth="1"/>
     <col min="17" max="17" width="12.1640625" style="4" customWidth="1"/>
-    <col min="18" max="18" width="31.83203125" style="5" customWidth="1"/>
-    <col min="19" max="19" width="29.5" style="5" customWidth="1"/>
-    <col min="20" max="20" width="18.83203125" style="6" customWidth="1"/>
-    <col min="21" max="21" width="18.33203125" style="6" customWidth="1"/>
-    <col min="22" max="22" width="15.33203125" style="7" customWidth="1"/>
-    <col min="23" max="23" width="16.33203125" style="7" customWidth="1"/>
-    <col min="24" max="24" width="40.6640625" style="7" customWidth="1"/>
-    <col min="25" max="25" width="30.6640625" style="7" customWidth="1"/>
-    <col min="26" max="26" width="15.83203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="34.1640625" style="7" customWidth="1"/>
-    <col min="28" max="28" width="16.5" style="7" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="35" style="7" customWidth="1"/>
-    <col min="30" max="16384" width="11.5" style="7"/>
+    <col min="18" max="19" width="31.83203125" style="5" customWidth="1"/>
+    <col min="20" max="20" width="29.5" style="5" customWidth="1"/>
+    <col min="21" max="21" width="18.83203125" style="6" customWidth="1"/>
+    <col min="22" max="22" width="18.33203125" style="6" customWidth="1"/>
+    <col min="23" max="23" width="15.33203125" style="7" customWidth="1"/>
+    <col min="24" max="24" width="16.33203125" style="7" customWidth="1"/>
+    <col min="25" max="25" width="40.6640625" style="7" customWidth="1"/>
+    <col min="26" max="26" width="30.6640625" style="7" customWidth="1"/>
+    <col min="27" max="27" width="15.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="34.1640625" style="7" customWidth="1"/>
+    <col min="29" max="29" width="16.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="35" style="7" customWidth="1"/>
+    <col min="31" max="16384" width="11.5" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:35" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="9"/>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
@@ -692,10 +695,11 @@
       <c r="Q1" s="9"/>
       <c r="R1" s="10"/>
       <c r="S1" s="10"/>
-      <c r="T1" s="11"/>
+      <c r="T1" s="10"/>
       <c r="U1" s="11"/>
-    </row>
-    <row r="2" spans="1:34" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="V1" s="11"/>
+    </row>
+    <row r="2" spans="1:35" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="17"/>
       <c r="B2" s="17"/>
       <c r="C2" s="17"/>
@@ -717,8 +721,9 @@
       <c r="S2" s="17"/>
       <c r="T2" s="17"/>
       <c r="U2" s="17"/>
-    </row>
-    <row r="3" spans="1:34" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="V2" s="17"/>
+    </row>
+    <row r="3" spans="1:35" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="17"/>
       <c r="B3" s="17"/>
       <c r="C3" s="17"/>
@@ -740,8 +745,9 @@
       <c r="S3" s="17"/>
       <c r="T3" s="17"/>
       <c r="U3" s="17"/>
-    </row>
-    <row r="4" spans="1:34" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="V3" s="17"/>
+    </row>
+    <row r="4" spans="1:35" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="9"/>
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
@@ -761,10 +767,11 @@
       <c r="Q4" s="14"/>
       <c r="R4" s="13"/>
       <c r="S4" s="13"/>
-      <c r="T4" s="11"/>
+      <c r="T4" s="13"/>
       <c r="U4" s="11"/>
-    </row>
-    <row r="5" spans="1:34" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="V4" s="11"/>
+    </row>
+    <row r="5" spans="1:35" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="9"/>
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
@@ -784,10 +791,11 @@
       <c r="Q5" s="9"/>
       <c r="R5" s="10"/>
       <c r="S5" s="10"/>
-      <c r="T5" s="11"/>
+      <c r="T5" s="10"/>
       <c r="U5" s="11"/>
-    </row>
-    <row r="6" spans="1:34" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="V5" s="11"/>
+    </row>
+    <row r="6" spans="1:35" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="9"/>
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
@@ -807,10 +815,11 @@
       <c r="Q6" s="9"/>
       <c r="R6" s="10"/>
       <c r="S6" s="10"/>
-      <c r="T6" s="11"/>
+      <c r="T6" s="10"/>
       <c r="U6" s="11"/>
-    </row>
-    <row r="7" spans="1:34" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="V6" s="11"/>
+    </row>
+    <row r="7" spans="1:35" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="9"/>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
@@ -830,10 +839,11 @@
       <c r="Q7" s="9"/>
       <c r="R7" s="10"/>
       <c r="S7" s="10"/>
-      <c r="T7" s="11"/>
+      <c r="T7" s="10"/>
       <c r="U7" s="11"/>
-    </row>
-    <row r="8" spans="1:34" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="V7" s="11"/>
+    </row>
+    <row r="8" spans="1:35" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="9"/>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
@@ -853,10 +863,11 @@
       <c r="Q8" s="9"/>
       <c r="R8" s="10"/>
       <c r="S8" s="10"/>
-      <c r="T8" s="11"/>
+      <c r="T8" s="10"/>
       <c r="U8" s="11"/>
-    </row>
-    <row r="9" spans="1:34" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="V8" s="11"/>
+    </row>
+    <row r="9" spans="1:35" s="12" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="9"/>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
@@ -876,10 +887,11 @@
       <c r="Q9" s="9"/>
       <c r="R9" s="10"/>
       <c r="S9" s="10"/>
-      <c r="T9" s="11"/>
+      <c r="T9" s="10"/>
       <c r="U9" s="11"/>
-    </row>
-    <row r="10" spans="1:34" customFormat="1" ht="19" x14ac:dyDescent="0.2">
+      <c r="V9" s="11"/>
+    </row>
+    <row r="10" spans="1:35" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
@@ -935,43 +947,46 @@
         <v>4</v>
       </c>
       <c r="S10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="T10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="T10" s="3" t="s">
+      <c r="U10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="U10" s="3" t="s">
+      <c r="V10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="V10" s="3" t="s">
+      <c r="W10" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="W10" s="3" t="s">
+      <c r="X10" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="X10" s="3" t="s">
+      <c r="Y10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="Y10" s="3" t="s">
+      <c r="Z10" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="Z10" s="3" t="s">
+      <c r="AA10" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AA10" s="3" t="s">
+      <c r="AB10" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AB10" s="3" t="s">
+      <c r="AC10" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AC10" s="3" t="s">
+      <c r="AD10" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AD10" s="3" t="s">
+      <c r="AE10" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:35" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -991,9 +1006,9 @@
       <c r="Q11" s="4"/>
       <c r="R11" s="5"/>
       <c r="S11" s="5"/>
-      <c r="T11" s="6"/>
+      <c r="T11" s="5"/>
       <c r="U11" s="6"/>
-      <c r="V11" s="7"/>
+      <c r="V11" s="6"/>
       <c r="W11" s="7"/>
       <c r="X11" s="7"/>
       <c r="Y11" s="7"/>
@@ -1006,8 +1021,9 @@
       <c r="AF11" s="7"/>
       <c r="AG11" s="7"/>
       <c r="AH11" s="7"/>
-    </row>
-    <row r="12" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AI11" s="7"/>
+    </row>
+    <row r="12" spans="1:35" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -1027,9 +1043,9 @@
       <c r="Q12" s="4"/>
       <c r="R12" s="5"/>
       <c r="S12" s="5"/>
-      <c r="T12" s="6"/>
+      <c r="T12" s="5"/>
       <c r="U12" s="6"/>
-      <c r="V12" s="7"/>
+      <c r="V12" s="6"/>
       <c r="W12" s="7"/>
       <c r="X12" s="7"/>
       <c r="Y12" s="7"/>
@@ -1042,8 +1058,9 @@
       <c r="AF12" s="7"/>
       <c r="AG12" s="7"/>
       <c r="AH12" s="7"/>
-    </row>
-    <row r="13" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AI12" s="7"/>
+    </row>
+    <row r="13" spans="1:35" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -1063,9 +1080,9 @@
       <c r="Q13" s="4"/>
       <c r="R13" s="5"/>
       <c r="S13" s="5"/>
-      <c r="T13" s="6"/>
+      <c r="T13" s="5"/>
       <c r="U13" s="6"/>
-      <c r="V13" s="7"/>
+      <c r="V13" s="6"/>
       <c r="W13" s="7"/>
       <c r="X13" s="7"/>
       <c r="Y13" s="7"/>
@@ -1078,8 +1095,9 @@
       <c r="AF13" s="7"/>
       <c r="AG13" s="7"/>
       <c r="AH13" s="7"/>
-    </row>
-    <row r="14" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AI13" s="7"/>
+    </row>
+    <row r="14" spans="1:35" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -1099,9 +1117,9 @@
       <c r="Q14" s="4"/>
       <c r="R14" s="5"/>
       <c r="S14" s="5"/>
-      <c r="T14" s="6"/>
+      <c r="T14" s="5"/>
       <c r="U14" s="6"/>
-      <c r="V14" s="7"/>
+      <c r="V14" s="6"/>
       <c r="W14" s="7"/>
       <c r="X14" s="7"/>
       <c r="Y14" s="7"/>
@@ -1114,8 +1132,9 @@
       <c r="AF14" s="7"/>
       <c r="AG14" s="7"/>
       <c r="AH14" s="7"/>
-    </row>
-    <row r="15" spans="1:34" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AI14" s="7"/>
+    </row>
+    <row r="15" spans="1:35" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -1135,9 +1154,9 @@
       <c r="Q15" s="4"/>
       <c r="R15" s="5"/>
       <c r="S15" s="5"/>
-      <c r="T15" s="6"/>
+      <c r="T15" s="5"/>
       <c r="U15" s="6"/>
-      <c r="V15" s="7"/>
+      <c r="V15" s="6"/>
       <c r="W15" s="7"/>
       <c r="X15" s="7"/>
       <c r="Y15" s="7"/>
@@ -1150,11 +1169,12 @@
       <c r="AF15" s="7"/>
       <c r="AG15" s="7"/>
       <c r="AH15" s="7"/>
+      <c r="AI15" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A2:U2"/>
-    <mergeCell ref="A3:U3"/>
+    <mergeCell ref="A2:V2"/>
+    <mergeCell ref="A3:V3"/>
   </mergeCells>
   <pageMargins left="0.70866141732283505" right="0.70866141732283505" top="0.74803149606299202" bottom="0.74803149606299202" header="0.31496062992126" footer="0.31496062992126"/>
   <pageSetup scale="28" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>